<commit_message>
created code to generate single gaussian wave data measured using electrodes that can move
</commit_message>
<xml_diff>
--- a/test_gaussian_data_10_400.xlsx
+++ b/test_gaussian_data_10_400.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candace_chung/Desktop/Candace Chung Files/ICL/Academics/Year 4/MSci Project/code/MSci_Atrial_Fib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B170079-628D-AC4B-A7B8-E72F5348B6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88381DFB-E04D-3243-A86F-2C10DE1B6129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
   <dimension ref="A1:P2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection sqref="A1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>